<commit_message>
use adorn_totals() in README, don't use two deprecated functions
</commit_message>
<xml_diff>
--- a/dirty_data.xlsx
+++ b/dirty_data.xlsx
@@ -1,7 +1,7 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="16925"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
@@ -58,7 +58,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="89" uniqueCount="52">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
   <si>
     <t>Teacher</t>
   </si>
@@ -178,9 +178,6 @@
   </si>
   <si>
     <t>Coach</t>
-  </si>
-  <si>
-    <t>TBD</t>
   </si>
   <si>
     <t>Theater</t>
@@ -637,7 +634,7 @@
   <dimension ref="A1:L18"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="I5" sqref="I5"/>
+      <selection activeCell="D13" sqref="D13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
@@ -668,7 +665,7 @@
         <v>5</v>
       </c>
       <c r="E1" s="7" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="F1" s="7" t="s">
         <v>6</v>
@@ -713,10 +710,10 @@
       </c>
       <c r="H2" s="1"/>
       <c r="I2" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J2" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L2" s="10"/>
     </row>
@@ -744,10 +741,10 @@
       </c>
       <c r="H3" s="1"/>
       <c r="I3" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J3" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="L3" s="10"/>
     </row>
@@ -775,10 +772,10 @@
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="J4" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="L4" s="10"/>
     </row>
@@ -807,10 +804,10 @@
       </c>
       <c r="H5" s="1"/>
       <c r="I5" t="s">
+        <v>44</v>
+      </c>
+      <c r="J5" t="s">
         <v>45</v>
-      </c>
-      <c r="J5" t="s">
-        <v>46</v>
       </c>
       <c r="L5" s="10"/>
     </row>
@@ -838,7 +835,7 @@
       </c>
       <c r="H6" s="1"/>
       <c r="I6" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L6" s="10"/>
     </row>
@@ -866,7 +863,7 @@
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J7" t="s">
         <v>36</v>
@@ -897,7 +894,7 @@
       </c>
       <c r="H8" s="1"/>
       <c r="I8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
       <c r="J8" t="s">
         <v>36</v>
@@ -932,7 +929,7 @@
       </c>
       <c r="H10" s="1"/>
       <c r="J10" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="L10" s="10"/>
     </row>
@@ -960,7 +957,7 @@
       </c>
       <c r="H11" s="1"/>
       <c r="I11" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="L11" s="10"/>
     </row>
@@ -975,7 +972,7 @@
         <v>39</v>
       </c>
       <c r="D12" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="E12" s="12">
         <v>42221</v>
@@ -989,7 +986,7 @@
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="L12" s="10"/>
     </row>
@@ -1003,9 +1000,6 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
-      <c r="D13" t="s">
-        <v>40</v>
-      </c>
       <c r="E13" s="12">
         <v>34700</v>
       </c>
@@ -1018,7 +1012,7 @@
       </c>
       <c r="H13" s="1"/>
       <c r="J13" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="L13" s="10"/>
     </row>
@@ -1046,7 +1040,7 @@
       </c>
       <c r="H14" s="1"/>
       <c r="I14" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="J14" t="s">
         <v>35</v>

</xml_diff>

<commit_message>
update README, index, and dirty_data.xlsx to have even dirtier data and show functions like convert_to_date()
</commit_message>
<xml_diff>
--- a/dirty_data.xlsx
+++ b/dirty_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SFirke\Documents\Bitbucket\janitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samfi\Documents\git\janitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB444C5E-7B9A-480F-B39E-0A59DC2E76A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6072"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam Firke</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>Teacher</t>
   </si>
@@ -211,13 +212,25 @@
   </si>
   <si>
     <t>Basketball</t>
+  </si>
+  <si>
+    <t>Active?</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Data most recently refreshed on:</t>
+  </si>
+  <si>
+    <t>Dec-27 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +273,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -281,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -298,11 +326,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -317,8 +392,13 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -630,94 +710,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.62890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.05078125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="12">
-        <v>39690</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -728,13 +787,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="12">
         <v>39690</v>
       </c>
       <c r="F3" s="2">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>30</v>
@@ -746,86 +805,95 @@
       <c r="J3" t="s">
         <v>40</v>
       </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="12">
-        <v>37118</v>
+        <v>28</v>
+      </c>
+      <c r="E4" s="14">
+        <v>43479</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="s">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
       </c>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" t="e">
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="14">
+        <v>37118</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="e">
         <f>MAX(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="E5" s="12">
-        <v>27515</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" s="12">
-        <v>41431</v>
+        <v>38572</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -837,40 +905,46 @@
       <c r="I6" t="s">
         <v>44</v>
       </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="12">
-        <v>11037</v>
+        <v>34</v>
+      </c>
+      <c r="E7" s="14">
+        <v>42791</v>
       </c>
       <c r="F7" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>52</v>
       </c>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -881,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="12">
         <v>11037</v>
@@ -899,55 +973,64 @@
       <c r="J8" t="s">
         <v>36</v>
       </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
       <c r="L8" s="10"/>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E9" s="13"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="12">
+        <v>11037</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="13"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="12">
-        <v>32994</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="J10" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="12">
-        <v>27919</v>
+        <v>35</v>
+      </c>
+      <c r="E11" s="14">
+        <v>36423</v>
       </c>
       <c r="F11" s="2">
         <v>0.5</v>
@@ -956,43 +1039,48 @@
         <v>38</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" t="s">
-        <v>44</v>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" t="s">
+        <v>52</v>
       </c>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E12" s="12">
-        <v>42221</v>
-      </c>
-      <c r="F12" t="e">
-        <f>VLOOKUP(A12,M:M,2, FALSE)</f>
-        <v>#N/A</v>
+        <v>27919</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.5</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="K12" t="s">
+        <v>52</v>
       </c>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -1000,8 +1088,11 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
       <c r="E13" s="12">
-        <v>34700</v>
+        <v>42221</v>
       </c>
       <c r="F13" t="e">
         <f>VLOOKUP(A13,M:M,2, FALSE)</f>
@@ -1011,57 +1102,95 @@
         <v>38</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="J13" t="s">
-        <v>48</v>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" t="s">
+        <v>52</v>
       </c>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E14" s="12">
-        <v>40071</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.8</v>
+        <v>34700</v>
+      </c>
+      <c r="F14" t="e">
+        <f>VLOOKUP(A14,M:M,2, FALSE)</f>
+        <v>#N/A</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="12">
+        <v>40071</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" t="s">
         <v>41</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H18" s="1"/>
     </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H19" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
update documentation, dirty data spreadsheet to show new(er) janitor functions (#418)
* include examples of clean_names features that rely on snakecase::to_any_case, like #271 and #283
* update README, index, and dirty_data.xlsx to have even dirtier data and show functions like convert_to_date()
</commit_message>
<xml_diff>
--- a/dirty_data.xlsx
+++ b/dirty_data.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="17329"/>
-  <workbookPr defaultThemeVersion="164011"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23426"/>
+  <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SFirke\Documents\Bitbucket\janitor\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\samfi\Documents\git\janitor\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AB444C5E-7B9A-480F-B39E-0A59DC2E76A7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="15528" windowHeight="6072"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="171027"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,12 +25,12 @@
 </file>
 
 <file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
-<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
   <authors>
     <author>Sam Firke</author>
   </authors>
   <commentList>
-    <comment ref="I1" authorId="0" shapeId="0">
+    <comment ref="I2" authorId="0" shapeId="0" xr:uid="{00000000-0006-0000-0000-000001000000}">
       <text>
         <r>
           <rPr>
@@ -58,7 +59,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="88" uniqueCount="51">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="55">
   <si>
     <t>Teacher</t>
   </si>
@@ -211,13 +212,25 @@
   </si>
   <si>
     <t>Basketball</t>
+  </si>
+  <si>
+    <t>Active?</t>
+  </si>
+  <si>
+    <t>YES</t>
+  </si>
+  <si>
+    <t>Data most recently refreshed on:</t>
+  </si>
+  <si>
+    <t>Dec-27 2020</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
-  <fonts count="6" x14ac:knownFonts="1">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -260,6 +273,21 @@
       <name val="Tahoma"/>
       <family val="2"/>
     </font>
+    <font>
+      <b/>
+      <sz val="15"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="14"/>
+      <color rgb="FF7030A0"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="4">
     <fill>
@@ -281,7 +309,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="6">
     <border>
       <left/>
       <right/>
@@ -298,11 +326,58 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thick">
+        <color theme="4"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="18">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
     <xf numFmtId="9" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -317,8 +392,13 @@
     <xf numFmtId="14" fontId="2" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
     <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="1" fontId="0" fillId="3" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Heading 1" xfId="1" builtinId="16"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -630,94 +710,73 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:L18"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+  <dimension ref="A1:L19"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="D13" sqref="D13"/>
+      <selection activeCell="M5" sqref="M5"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.55000000000000004"/>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="10.89453125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="9.15625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.26171875" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="12.89453125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="8.3125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.15625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="8.62890625" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="13.05078125" bestFit="1" customWidth="1"/>
-    <col min="9" max="10" width="10.68359375" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="10.3125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="10.90625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="9.1796875" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="18.1796875" customWidth="1"/>
+    <col min="4" max="4" width="13.90625" customWidth="1"/>
+    <col min="5" max="5" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.1796875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.6328125" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="9" max="10" width="10.6328125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="10.26953125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="A1" s="7" t="s">
+    <row r="1" spans="1:12" ht="20" thickBot="1" x14ac:dyDescent="0.5">
+      <c r="A1" s="15" t="s">
+        <v>53</v>
+      </c>
+      <c r="B1" s="16"/>
+      <c r="C1" s="16"/>
+      <c r="D1" s="17" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="2" spans="1:12" s="9" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="A2" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B2" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="C1" s="7" t="s">
+      <c r="C2" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="7" t="s">
+      <c r="D2" s="7" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="7" t="s">
+      <c r="E2" s="7" t="s">
         <v>49</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="F2" s="7" t="s">
         <v>6</v>
       </c>
-      <c r="G1" s="7" t="s">
+      <c r="G2" s="7" t="s">
         <v>29</v>
       </c>
-      <c r="H1" s="8" t="s">
+      <c r="H2" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="I1" s="7" t="s">
+      <c r="I2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="J1" s="7" t="s">
+      <c r="J2" s="7" t="s">
         <v>1</v>
       </c>
-      <c r="K1" s="7" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A2" t="s">
-        <v>8</v>
-      </c>
-      <c r="B2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C2" t="s">
-        <v>0</v>
-      </c>
-      <c r="D2" t="s">
-        <v>27</v>
-      </c>
-      <c r="E2" s="12">
-        <v>39690</v>
-      </c>
-      <c r="F2" s="2">
-        <v>0.75</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>30</v>
-      </c>
-      <c r="H2" s="1"/>
-      <c r="I2" t="s">
-        <v>42</v>
-      </c>
-      <c r="J2" t="s">
-        <v>40</v>
-      </c>
-      <c r="L2" s="10"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K2" s="7" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>8</v>
       </c>
@@ -728,13 +787,13 @@
         <v>0</v>
       </c>
       <c r="D3" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="E3" s="12">
         <v>39690</v>
       </c>
       <c r="F3" s="2">
-        <v>0.25</v>
+        <v>0.75</v>
       </c>
       <c r="G3" s="6" t="s">
         <v>30</v>
@@ -746,86 +805,95 @@
       <c r="J3" t="s">
         <v>40</v>
       </c>
+      <c r="K3" t="s">
+        <v>52</v>
+      </c>
       <c r="L3" s="10"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
       <c r="B4" t="s">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="C4" t="s">
         <v>0</v>
       </c>
       <c r="D4" t="s">
-        <v>31</v>
-      </c>
-      <c r="E4" s="12">
-        <v>37118</v>
+        <v>28</v>
+      </c>
+      <c r="E4" s="14">
+        <v>43479</v>
       </c>
       <c r="F4" s="2">
-        <v>1</v>
-      </c>
-      <c r="G4" s="3" t="s">
+        <v>0.25</v>
+      </c>
+      <c r="G4" s="6" t="s">
         <v>30</v>
       </c>
       <c r="H4" s="1"/>
       <c r="I4" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="J4" t="s">
-        <v>41</v>
+        <v>40</v>
+      </c>
+      <c r="K4" t="s">
+        <v>52</v>
       </c>
       <c r="L4" s="10"/>
     </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="5" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>24</v>
+        <v>10</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C5" t="s">
         <v>0</v>
       </c>
-      <c r="D5" t="e">
+      <c r="D5" t="s">
+        <v>31</v>
+      </c>
+      <c r="E5" s="14">
+        <v>37118</v>
+      </c>
+      <c r="F5" s="2">
+        <v>1</v>
+      </c>
+      <c r="G5" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H5" s="1"/>
+      <c r="I5" t="s">
+        <v>43</v>
+      </c>
+      <c r="J5" t="s">
+        <v>41</v>
+      </c>
+      <c r="K5" t="s">
+        <v>52</v>
+      </c>
+      <c r="L5" s="10"/>
+    </row>
+    <row r="6" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>24</v>
+      </c>
+      <c r="B6" t="s">
+        <v>25</v>
+      </c>
+      <c r="C6" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" t="e">
         <f>MAX(#REF!)</f>
         <v>#REF!</v>
       </c>
-      <c r="E5" s="12">
-        <v>27515</v>
-      </c>
-      <c r="F5" s="2">
-        <v>1</v>
-      </c>
-      <c r="G5" s="3" t="s">
-        <v>30</v>
-      </c>
-      <c r="H5" s="1"/>
-      <c r="I5" t="s">
-        <v>44</v>
-      </c>
-      <c r="J5" t="s">
-        <v>45</v>
-      </c>
-      <c r="L5" s="10"/>
-    </row>
-    <row r="6" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A6" t="s">
-        <v>14</v>
-      </c>
-      <c r="B6" t="s">
-        <v>15</v>
-      </c>
-      <c r="C6" t="s">
-        <v>33</v>
-      </c>
-      <c r="D6" t="s">
-        <v>34</v>
-      </c>
       <c r="E6" s="12">
-        <v>41431</v>
+        <v>38572</v>
       </c>
       <c r="F6" s="2">
         <v>1</v>
@@ -837,40 +905,46 @@
       <c r="I6" t="s">
         <v>44</v>
       </c>
+      <c r="J6" t="s">
+        <v>45</v>
+      </c>
+      <c r="K6" t="s">
+        <v>52</v>
+      </c>
       <c r="L6" s="10"/>
     </row>
-    <row r="7" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="7" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>22</v>
+        <v>14</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="C7" t="s">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="D7" t="s">
-        <v>36</v>
-      </c>
-      <c r="E7" s="12">
-        <v>11037</v>
+        <v>34</v>
+      </c>
+      <c r="E7" s="14">
+        <v>42791</v>
       </c>
       <c r="F7" s="2">
-        <v>0.5</v>
+        <v>1</v>
       </c>
       <c r="G7" s="3" t="s">
         <v>30</v>
       </c>
       <c r="H7" s="1"/>
       <c r="I7" t="s">
-        <v>46</v>
-      </c>
-      <c r="J7" t="s">
-        <v>36</v>
+        <v>44</v>
+      </c>
+      <c r="K7" t="s">
+        <v>52</v>
       </c>
       <c r="L7" s="10"/>
     </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="8" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>22</v>
       </c>
@@ -881,7 +955,7 @@
         <v>0</v>
       </c>
       <c r="D8" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="E8" s="12">
         <v>11037</v>
@@ -899,55 +973,64 @@
       <c r="J8" t="s">
         <v>36</v>
       </c>
+      <c r="K8" t="s">
+        <v>52</v>
+      </c>
       <c r="L8" s="10"/>
     </row>
-    <row r="9" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.55000000000000004">
-      <c r="E9" s="13"/>
-      <c r="L9" s="11"/>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A10" t="s">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
+      </c>
+      <c r="C9" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" t="s">
+        <v>37</v>
+      </c>
+      <c r="E9" s="12">
+        <v>11037</v>
+      </c>
+      <c r="F9" s="2">
+        <v>0.5</v>
+      </c>
+      <c r="G9" s="3" t="s">
+        <v>30</v>
+      </c>
+      <c r="H9" s="1"/>
+      <c r="I9" t="s">
+        <v>46</v>
+      </c>
+      <c r="J9" t="s">
+        <v>36</v>
+      </c>
+      <c r="K9" t="s">
+        <v>52</v>
+      </c>
+      <c r="L9" s="10"/>
+    </row>
+    <row r="10" spans="1:12" s="4" customFormat="1" x14ac:dyDescent="0.35">
+      <c r="E10" s="13"/>
+      <c r="L10" s="11"/>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>18</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B11" t="s">
         <v>19</v>
-      </c>
-      <c r="C10" t="s">
-        <v>0</v>
-      </c>
-      <c r="D10" t="s">
-        <v>35</v>
-      </c>
-      <c r="E10" s="12">
-        <v>32994</v>
-      </c>
-      <c r="F10" s="2">
-        <v>0.5</v>
-      </c>
-      <c r="G10" s="5" t="s">
-        <v>38</v>
-      </c>
-      <c r="H10" s="1"/>
-      <c r="J10" t="s">
-        <v>47</v>
-      </c>
-      <c r="L10" s="10"/>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="A11" t="s">
-        <v>20</v>
-      </c>
-      <c r="B11" t="s">
-        <v>21</v>
       </c>
       <c r="C11" t="s">
         <v>0</v>
       </c>
       <c r="D11" t="s">
-        <v>32</v>
-      </c>
-      <c r="E11" s="12">
-        <v>27919</v>
+        <v>35</v>
+      </c>
+      <c r="E11" s="14">
+        <v>36423</v>
       </c>
       <c r="F11" s="2">
         <v>0.5</v>
@@ -956,43 +1039,48 @@
         <v>38</v>
       </c>
       <c r="H11" s="1"/>
-      <c r="I11" t="s">
-        <v>44</v>
+      <c r="J11" t="s">
+        <v>47</v>
+      </c>
+      <c r="K11" t="s">
+        <v>52</v>
       </c>
       <c r="L11" s="10"/>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>26</v>
+        <v>20</v>
       </c>
       <c r="B12" t="s">
-        <v>13</v>
+        <v>21</v>
       </c>
       <c r="C12" t="s">
-        <v>39</v>
+        <v>0</v>
       </c>
       <c r="D12" t="s">
-        <v>50</v>
+        <v>32</v>
       </c>
       <c r="E12" s="12">
-        <v>42221</v>
-      </c>
-      <c r="F12" t="e">
-        <f>VLOOKUP(A12,M:M,2, FALSE)</f>
-        <v>#N/A</v>
+        <v>27919</v>
+      </c>
+      <c r="F12" s="2">
+        <v>0.5</v>
       </c>
       <c r="G12" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H12" s="1"/>
       <c r="I12" t="s">
-        <v>42</v>
+        <v>44</v>
+      </c>
+      <c r="K12" t="s">
+        <v>52</v>
       </c>
       <c r="L12" s="10"/>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
-        <v>12</v>
+        <v>26</v>
       </c>
       <c r="B13" t="s">
         <v>13</v>
@@ -1000,8 +1088,11 @@
       <c r="C13" t="s">
         <v>39</v>
       </c>
+      <c r="D13" t="s">
+        <v>50</v>
+      </c>
       <c r="E13" s="12">
-        <v>34700</v>
+        <v>42221</v>
       </c>
       <c r="F13" t="e">
         <f>VLOOKUP(A13,M:M,2, FALSE)</f>
@@ -1011,57 +1102,95 @@
         <v>38</v>
       </c>
       <c r="H13" s="1"/>
-      <c r="J13" t="s">
-        <v>48</v>
+      <c r="I13" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" t="s">
+        <v>52</v>
       </c>
       <c r="L13" s="10"/>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.35">
       <c r="A14" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="B14" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" t="s">
-        <v>35</v>
+        <v>39</v>
       </c>
       <c r="E14" s="12">
-        <v>40071</v>
-      </c>
-      <c r="F14" s="2">
-        <v>0.8</v>
+        <v>34700</v>
+      </c>
+      <c r="F14" t="e">
+        <f>VLOOKUP(A14,M:M,2, FALSE)</f>
+        <v>#N/A</v>
       </c>
       <c r="G14" s="5" t="s">
         <v>38</v>
       </c>
       <c r="H14" s="1"/>
-      <c r="I14" t="s">
+      <c r="J14" t="s">
+        <v>48</v>
+      </c>
+      <c r="K14" t="s">
+        <v>52</v>
+      </c>
+      <c r="L14" s="10"/>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>16</v>
+      </c>
+      <c r="B15" t="s">
+        <v>17</v>
+      </c>
+      <c r="C15" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" t="s">
+        <v>35</v>
+      </c>
+      <c r="E15" s="12">
+        <v>40071</v>
+      </c>
+      <c r="F15" s="2">
+        <v>0.8</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H15" s="1"/>
+      <c r="I15" t="s">
         <v>41</v>
       </c>
-      <c r="J14" t="s">
+      <c r="J15" t="s">
         <v>35</v>
       </c>
-      <c r="L14" s="10"/>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.55000000000000004">
-      <c r="H15" s="1"/>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.55000000000000004">
+      <c r="K15" t="s">
+        <v>52</v>
+      </c>
+      <c r="L15" s="10"/>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.35">
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="17" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="8:8" x14ac:dyDescent="0.55000000000000004">
+    <row r="18" spans="8:8" x14ac:dyDescent="0.35">
       <c r="H18" s="1"/>
     </row>
+    <row r="19" spans="8:8" x14ac:dyDescent="0.35">
+      <c r="H19" s="1"/>
+    </row>
   </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:C1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="4294967293" r:id="rId1"/>
   <legacyDrawing r:id="rId2"/>
 </worksheet>
 </file>
</xml_diff>